<commit_message>
allow to update existing items. using new excel template
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspaces\LCMedicalAssurancePolicyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210A4A3C-F117-4604-AD25-577F79D7F827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BF58E-07DC-4B6D-8FFF-0390C59F2BCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19092" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="57" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="58" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$C$3:$W$224</definedName>
@@ -340,7 +341,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9347" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9489" uniqueCount="530">
   <si>
     <t>省份</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1989,12 +1990,309 @@
   <si>
     <t>Id</t>
   </si>
+  <si>
+    <t>商品类别</t>
+  </si>
+  <si>
+    <t>区域</t>
+  </si>
+  <si>
+    <t>省份</t>
+  </si>
+  <si>
+    <t>统筹区</t>
+  </si>
+  <si>
+    <t>重点城市</t>
+  </si>
+  <si>
+    <t>参保人群</t>
+  </si>
+  <si>
+    <t>类别</t>
+  </si>
+  <si>
+    <t>病种名称-标准</t>
+  </si>
+  <si>
+    <t>病种名称-实际</t>
+  </si>
+  <si>
+    <t>医院级别</t>
+  </si>
+  <si>
+    <t>保险类型</t>
+  </si>
+  <si>
+    <t>首自付(两病)</t>
+  </si>
+  <si>
+    <t>起付线(两病)</t>
+  </si>
+  <si>
+    <t>报销比例(两病)</t>
+  </si>
+  <si>
+    <t>报销限额-元/年(两病)</t>
+  </si>
+  <si>
+    <t>保险类型（普通门诊）</t>
+  </si>
+  <si>
+    <t>待遇类型（普通门诊）</t>
+  </si>
+  <si>
+    <t>首自付（普通门诊）</t>
+  </si>
+  <si>
+    <t>起付线-元/年（普通门诊）</t>
+  </si>
+  <si>
+    <t>报销比例（普通门诊）</t>
+  </si>
+  <si>
+    <t>报销限额-元/年（普通门诊）</t>
+  </si>
+  <si>
+    <t>保险类型（门特）</t>
+  </si>
+  <si>
+    <t>产品政策类型-标准化（门特）</t>
+  </si>
+  <si>
+    <t>产品政策类型-实际（门特）</t>
+  </si>
+  <si>
+    <t>首自付（门特）</t>
+  </si>
+  <si>
+    <t>起付线（门特）</t>
+  </si>
+  <si>
+    <t>报销比例/额度区间（门特）</t>
+  </si>
+  <si>
+    <t>报销限额-元/年（门特）</t>
+  </si>
+  <si>
+    <t>备注（门特）</t>
+  </si>
+  <si>
+    <t>发文时间（门特）</t>
+  </si>
+  <si>
+    <t>文件链接（门特）</t>
+  </si>
+  <si>
+    <t>住院报销待遇</t>
+  </si>
+  <si>
+    <t>政策叠加情况（G-U列）</t>
+  </si>
+  <si>
+    <t>保险类型（双通道）</t>
+  </si>
+  <si>
+    <t>是否双通道（双通道）</t>
+  </si>
+  <si>
+    <t>双通道目录结构（双通道）</t>
+  </si>
+  <si>
+    <t>双通道定点药店数（双通道）</t>
+  </si>
+  <si>
+    <t>三定/五定及其他要求（双通道）</t>
+  </si>
+  <si>
+    <t>备注（双通道）</t>
+  </si>
+  <si>
+    <t>主要竞品备注</t>
+  </si>
+  <si>
+    <t>GoodsCategory</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>WholeArea</t>
+  </si>
+  <si>
+    <t>KeyCity</t>
+  </si>
+  <si>
+    <t>InsuredCrowd</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>StandardDiseaseName</t>
+  </si>
+  <si>
+    <t>ActualDiseaseName</t>
+  </si>
+  <si>
+    <t>HospitalLevel</t>
+  </si>
+  <si>
+    <t>InsuranceType</t>
+  </si>
+  <si>
+    <t>FirstPayDisease</t>
+  </si>
+  <si>
+    <t>StartingLineDisease</t>
+  </si>
+  <si>
+    <t>ReimbursementRatioDisease</t>
+  </si>
+  <si>
+    <t>ReimbursementLimitsDisease</t>
+  </si>
+  <si>
+    <t>InsuranceTypeOne</t>
+  </si>
+  <si>
+    <t>TreatmentType</t>
+  </si>
+  <si>
+    <t>FirstPayOutpatient</t>
+  </si>
+  <si>
+    <t>StartingLineOutpatient</t>
+  </si>
+  <si>
+    <t>ReimbursementRatioOutpatient</t>
+  </si>
+  <si>
+    <t>ReimbursementLimitsOutpatient</t>
+  </si>
+  <si>
+    <t>InsuranceTypeTwo</t>
+  </si>
+  <si>
+    <t>ProductPolicyTypeStandard</t>
+  </si>
+  <si>
+    <t>ProductPolicyTypeActual</t>
+  </si>
+  <si>
+    <t>FirstPay</t>
+  </si>
+  <si>
+    <t>StartingLine</t>
+  </si>
+  <si>
+    <t>ReimbursementRatio</t>
+  </si>
+  <si>
+    <t>ReimbursementLimits</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>DispatchTime</t>
+  </si>
+  <si>
+    <t>FileLink</t>
+  </si>
+  <si>
+    <t>ReimbursementHospitalization</t>
+  </si>
+  <si>
+    <t>PolicyCverlay</t>
+  </si>
+  <si>
+    <t>InsuranceTypeThree</t>
+  </si>
+  <si>
+    <t>IsDualChannel</t>
+  </si>
+  <si>
+    <t>TwoChannelStructure</t>
+  </si>
+  <si>
+    <t>FixedPointPharmacy</t>
+  </si>
+  <si>
+    <t>OtherRequirements</t>
+  </si>
+  <si>
+    <t>TwoChannelRemark</t>
+  </si>
+  <si>
+    <t>CompetitiveProductsRemark</t>
+  </si>
+  <si>
+    <t>乙类药品-住院</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>江苏</t>
+  </si>
+  <si>
+    <t>省直</t>
+  </si>
+  <si>
+    <t>住院</t>
+  </si>
+  <si>
+    <t>0%-30%</t>
+  </si>
+  <si>
+    <t>70%-100%</t>
+  </si>
+  <si>
+    <t>无</t>
+  </si>
+  <si>
+    <t>参照南京职工报销比例</t>
+  </si>
+  <si>
+    <t>无公开发文</t>
+  </si>
+  <si>
+    <t>乙类-门诊</t>
+  </si>
+  <si>
+    <t>上海</t>
+  </si>
+  <si>
+    <t>糖尿病</t>
+  </si>
+  <si>
+    <t>门诊统筹</t>
+  </si>
+  <si>
+    <t>门慢、门特</t>
+  </si>
+  <si>
+    <t>参保待遇查询小项 (sh.gov.cn)</t>
+  </si>
+  <si>
+    <t>双通道</t>
+  </si>
+  <si>
+    <t>度易达</t>
+  </si>
+  <si>
+    <t>两病</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2081,10 +2379,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2308,7 +2615,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2483,6 +2790,9 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2525,9 +2835,9 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2845,121 +3155,121 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8900981E-E299-424C-9524-4C3B502A9E21}">
   <dimension ref="A1:Y666"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="9" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:A3"/>
+      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="9"/>
-    <col min="2" max="2" width="9.5703125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" style="9" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" style="9" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="10"/>
-    <col min="13" max="13" width="8.85546875" style="9"/>
-    <col min="14" max="14" width="8.85546875" style="10"/>
-    <col min="15" max="16" width="9.85546875" style="9" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="9" customWidth="1"/>
-    <col min="18" max="23" width="8.85546875" style="9"/>
-    <col min="24" max="24" width="21.85546875" style="9" customWidth="1"/>
-    <col min="25" max="16384" width="8.85546875" style="9"/>
+    <col min="1" max="1" width="8.88671875" style="9"/>
+    <col min="2" max="2" width="9.5546875" style="9" customWidth="1"/>
+    <col min="3" max="3" width="2.88671875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="5.109375" style="9" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="15.109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="10"/>
+    <col min="13" max="13" width="8.88671875" style="9"/>
+    <col min="14" max="14" width="8.88671875" style="10"/>
+    <col min="15" max="16" width="9.88671875" style="9" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" style="9" customWidth="1"/>
+    <col min="18" max="23" width="8.88671875" style="9"/>
+    <col min="24" max="24" width="21.88671875" style="9" customWidth="1"/>
+    <col min="25" max="16384" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="83.45" customHeight="1">
-      <c r="C1" s="60" t="s">
+    <row r="1" spans="1:23" ht="83.4" customHeight="1">
+      <c r="C1" s="61" t="s">
         <v>400</v>
       </c>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61"/>
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
     </row>
     <row r="2" spans="1:23" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="60" t="s">
         <v>430</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="60" t="s">
         <v>426</v>
       </c>
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="67" t="s">
+      <c r="D2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="67" t="s">
+      <c r="E2" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="67" t="s">
+      <c r="F2" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="H2" s="67" t="s">
+      <c r="H2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="65" t="s">
+      <c r="I2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="71" t="s">
+      <c r="J2" s="72" t="s">
         <v>151</v>
       </c>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="72"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="72"/>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="69" t="s">
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="70" t="s">
         <v>154</v>
       </c>
-      <c r="R2" s="61" t="s">
+      <c r="R2" s="62" t="s">
         <v>152</v>
       </c>
-      <c r="S2" s="61"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="61"/>
-      <c r="V2" s="62"/>
-      <c r="W2" s="63" t="s">
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="64" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="23.45" customHeight="1">
-      <c r="A3" s="74"/>
-      <c r="B3" s="74"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="66"/>
+    <row r="3" spans="1:23" s="2" customFormat="1" ht="23.4" customHeight="1">
+      <c r="A3" s="60"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="67"/>
       <c r="J3" s="7" t="s">
         <v>14</v>
       </c>
@@ -2981,7 +3291,7 @@
       <c r="P3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="Q3" s="70"/>
+      <c r="Q3" s="71"/>
       <c r="R3" s="3" t="s">
         <v>153</v>
       </c>
@@ -2997,7 +3307,7 @@
       <c r="V3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="64"/>
+      <c r="W3" s="65"/>
     </row>
     <row r="4" spans="1:23" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="5">
@@ -3129,7 +3439,7 @@
       <c r="V5" s="16"/>
       <c r="W5" s="16"/>
     </row>
-    <row r="6" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="6" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -3192,7 +3502,7 @@
       <c r="V6" s="16"/>
       <c r="W6" s="16"/>
     </row>
-    <row r="7" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="7" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A7" s="5">
         <v>4</v>
       </c>
@@ -3257,7 +3567,7 @@
       <c r="V7" s="16"/>
       <c r="W7" s="16"/>
     </row>
-    <row r="8" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="8" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A8" s="5">
         <v>5</v>
       </c>
@@ -3322,7 +3632,7 @@
       <c r="V8" s="16"/>
       <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="9" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -3387,7 +3697,7 @@
       <c r="V9" s="16"/>
       <c r="W9" s="16"/>
     </row>
-    <row r="10" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="10" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A10" s="5">
         <v>7</v>
       </c>
@@ -3452,7 +3762,7 @@
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
     </row>
-    <row r="11" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="11" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A11" s="5">
         <v>8</v>
       </c>
@@ -3517,7 +3827,7 @@
       <c r="V11" s="16"/>
       <c r="W11" s="16"/>
     </row>
-    <row r="12" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="12" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A12" s="5">
         <v>9</v>
       </c>
@@ -3582,7 +3892,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="13" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A13" s="5">
         <v>10</v>
       </c>
@@ -3647,7 +3957,7 @@
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
     </row>
-    <row r="14" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="14" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A14" s="5">
         <v>11</v>
       </c>
@@ -3712,7 +4022,7 @@
       <c r="V14" s="16"/>
       <c r="W14" s="16"/>
     </row>
-    <row r="15" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="15" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A15" s="5">
         <v>12</v>
       </c>
@@ -3777,7 +4087,7 @@
       <c r="V15" s="16"/>
       <c r="W15" s="16"/>
     </row>
-    <row r="16" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="16" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A16" s="5">
         <v>13</v>
       </c>
@@ -3842,7 +4152,7 @@
       <c r="V16" s="16"/>
       <c r="W16" s="16"/>
     </row>
-    <row r="17" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="17" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A17" s="5">
         <v>14</v>
       </c>
@@ -3907,7 +4217,7 @@
       <c r="V17" s="16"/>
       <c r="W17" s="16"/>
     </row>
-    <row r="18" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="18" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A18" s="5">
         <v>15</v>
       </c>
@@ -3972,7 +4282,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="16"/>
     </row>
-    <row r="19" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="19" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A19" s="5">
         <v>16</v>
       </c>
@@ -4035,7 +4345,7 @@
       <c r="V19" s="16"/>
       <c r="W19" s="16"/>
     </row>
-    <row r="20" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="20" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A20" s="5">
         <v>17</v>
       </c>
@@ -4098,7 +4408,7 @@
       <c r="V20" s="16"/>
       <c r="W20" s="16"/>
     </row>
-    <row r="21" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="21" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A21" s="5">
         <v>18</v>
       </c>
@@ -4161,7 +4471,7 @@
       <c r="V21" s="16"/>
       <c r="W21" s="16"/>
     </row>
-    <row r="22" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="22" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A22" s="5">
         <v>19</v>
       </c>
@@ -4224,7 +4534,7 @@
       <c r="V22" s="16"/>
       <c r="W22" s="16"/>
     </row>
-    <row r="23" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="23" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A23" s="5">
         <v>20</v>
       </c>
@@ -4289,7 +4599,7 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
     </row>
-    <row r="24" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="24" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A24" s="5">
         <v>21</v>
       </c>
@@ -4354,7 +4664,7 @@
       <c r="V24" s="16"/>
       <c r="W24" s="16"/>
     </row>
-    <row r="25" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="25" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A25" s="5">
         <v>22</v>
       </c>
@@ -4417,7 +4727,7 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
     </row>
-    <row r="26" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="26" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A26" s="5">
         <v>23</v>
       </c>
@@ -4480,7 +4790,7 @@
       <c r="V26" s="16"/>
       <c r="W26" s="16"/>
     </row>
-    <row r="27" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="27" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A27" s="5">
         <v>24</v>
       </c>
@@ -4545,7 +4855,7 @@
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
     </row>
-    <row r="28" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="28" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A28" s="5">
         <v>25</v>
       </c>
@@ -17274,7 +17584,7 @@
       <c r="V226" s="16"/>
       <c r="W226" s="16"/>
     </row>
-    <row r="227" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="227" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A227" s="5">
         <v>224</v>
       </c>
@@ -17337,7 +17647,7 @@
       <c r="V227" s="16"/>
       <c r="W227" s="16"/>
     </row>
-    <row r="228" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="228" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A228" s="5">
         <v>225</v>
       </c>
@@ -17400,7 +17710,7 @@
       <c r="V228" s="16"/>
       <c r="W228" s="16"/>
     </row>
-    <row r="229" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="229" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A229" s="5">
         <v>226</v>
       </c>
@@ -17463,7 +17773,7 @@
       <c r="V229" s="16"/>
       <c r="W229" s="16"/>
     </row>
-    <row r="230" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="230" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A230" s="5">
         <v>227</v>
       </c>
@@ -17526,7 +17836,7 @@
       <c r="V230" s="16"/>
       <c r="W230" s="16"/>
     </row>
-    <row r="231" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="231" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A231" s="5">
         <v>228</v>
       </c>
@@ -17589,7 +17899,7 @@
       <c r="V231" s="16"/>
       <c r="W231" s="16"/>
     </row>
-    <row r="232" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="232" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A232" s="5">
         <v>229</v>
       </c>
@@ -17652,7 +17962,7 @@
       <c r="V232" s="16"/>
       <c r="W232" s="16"/>
     </row>
-    <row r="233" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="233" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A233" s="5">
         <v>230</v>
       </c>
@@ -17715,7 +18025,7 @@
       <c r="V233" s="16"/>
       <c r="W233" s="16"/>
     </row>
-    <row r="234" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="234" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A234" s="5">
         <v>231</v>
       </c>
@@ -17778,7 +18088,7 @@
       <c r="V234" s="16"/>
       <c r="W234" s="16"/>
     </row>
-    <row r="235" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="235" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A235" s="5">
         <v>232</v>
       </c>
@@ -17841,7 +18151,7 @@
       <c r="V235" s="16"/>
       <c r="W235" s="16"/>
     </row>
-    <row r="236" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="236" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A236" s="5">
         <v>233</v>
       </c>
@@ -17904,7 +18214,7 @@
       <c r="V236" s="16"/>
       <c r="W236" s="16"/>
     </row>
-    <row r="237" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="237" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A237" s="5">
         <v>234</v>
       </c>
@@ -17967,7 +18277,7 @@
       <c r="V237" s="16"/>
       <c r="W237" s="16"/>
     </row>
-    <row r="238" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="238" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A238" s="5">
         <v>235</v>
       </c>
@@ -18030,7 +18340,7 @@
       <c r="V238" s="16"/>
       <c r="W238" s="16"/>
     </row>
-    <row r="239" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="239" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A239" s="5">
         <v>236</v>
       </c>
@@ -18093,7 +18403,7 @@
       <c r="V239" s="16"/>
       <c r="W239" s="16"/>
     </row>
-    <row r="240" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="240" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A240" s="5">
         <v>237</v>
       </c>
@@ -18156,7 +18466,7 @@
       <c r="V240" s="16"/>
       <c r="W240" s="16"/>
     </row>
-    <row r="241" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="241" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A241" s="5">
         <v>238</v>
       </c>
@@ -18219,7 +18529,7 @@
       <c r="V241" s="16"/>
       <c r="W241" s="16"/>
     </row>
-    <row r="242" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="242" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A242" s="5">
         <v>239</v>
       </c>
@@ -18282,7 +18592,7 @@
       <c r="V242" s="16"/>
       <c r="W242" s="16"/>
     </row>
-    <row r="243" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="243" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A243" s="5">
         <v>240</v>
       </c>
@@ -18345,7 +18655,7 @@
       <c r="V243" s="16"/>
       <c r="W243" s="16"/>
     </row>
-    <row r="244" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="244" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A244" s="5">
         <v>241</v>
       </c>
@@ -18408,7 +18718,7 @@
       <c r="V244" s="16"/>
       <c r="W244" s="16"/>
     </row>
-    <row r="245" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="245" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A245" s="5">
         <v>242</v>
       </c>
@@ -18471,7 +18781,7 @@
       <c r="V245" s="16"/>
       <c r="W245" s="16"/>
     </row>
-    <row r="246" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="246" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A246" s="5">
         <v>243</v>
       </c>
@@ -18534,7 +18844,7 @@
       <c r="V246" s="16"/>
       <c r="W246" s="16"/>
     </row>
-    <row r="247" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="247" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A247" s="5">
         <v>244</v>
       </c>
@@ -18597,7 +18907,7 @@
       <c r="V247" s="16"/>
       <c r="W247" s="16"/>
     </row>
-    <row r="248" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="248" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A248" s="5">
         <v>245</v>
       </c>
@@ -18660,7 +18970,7 @@
       <c r="V248" s="16"/>
       <c r="W248" s="16"/>
     </row>
-    <row r="249" spans="1:24" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="249" spans="1:24" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A249" s="5">
         <v>246</v>
       </c>
@@ -31222,7 +31532,7 @@
       <c r="V447" s="16"/>
       <c r="W447" s="16"/>
     </row>
-    <row r="448" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="448" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A448" s="5">
         <v>445</v>
       </c>
@@ -31285,7 +31595,7 @@
       <c r="V448" s="16"/>
       <c r="W448" s="16"/>
     </row>
-    <row r="449" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="449" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A449" s="5">
         <v>446</v>
       </c>
@@ -31350,7 +31660,7 @@
       <c r="V449" s="16"/>
       <c r="W449" s="16"/>
     </row>
-    <row r="450" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="450" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A450" s="5">
         <v>447</v>
       </c>
@@ -31415,7 +31725,7 @@
       <c r="V450" s="16"/>
       <c r="W450" s="16"/>
     </row>
-    <row r="451" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="451" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A451" s="5">
         <v>448</v>
       </c>
@@ -31480,7 +31790,7 @@
       <c r="V451" s="16"/>
       <c r="W451" s="16"/>
     </row>
-    <row r="452" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="452" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A452" s="5">
         <v>449</v>
       </c>
@@ -31545,7 +31855,7 @@
       <c r="V452" s="16"/>
       <c r="W452" s="16"/>
     </row>
-    <row r="453" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="453" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A453" s="5">
         <v>450</v>
       </c>
@@ -31608,7 +31918,7 @@
       <c r="V453" s="16"/>
       <c r="W453" s="16"/>
     </row>
-    <row r="454" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="454" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A454" s="5">
         <v>451</v>
       </c>
@@ -31671,7 +31981,7 @@
       <c r="V454" s="16"/>
       <c r="W454" s="16"/>
     </row>
-    <row r="455" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="455" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A455" s="5">
         <v>452</v>
       </c>
@@ -31736,7 +32046,7 @@
       <c r="V455" s="16"/>
       <c r="W455" s="16"/>
     </row>
-    <row r="456" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="456" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A456" s="5">
         <v>453</v>
       </c>
@@ -31801,7 +32111,7 @@
       <c r="V456" s="16"/>
       <c r="W456" s="16"/>
     </row>
-    <row r="457" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="457" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A457" s="5">
         <v>454</v>
       </c>
@@ -31866,7 +32176,7 @@
       <c r="V457" s="16"/>
       <c r="W457" s="16"/>
     </row>
-    <row r="458" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="458" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A458" s="5">
         <v>455</v>
       </c>
@@ -31931,7 +32241,7 @@
       <c r="V458" s="16"/>
       <c r="W458" s="16"/>
     </row>
-    <row r="459" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="459" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A459" s="5">
         <v>456</v>
       </c>
@@ -31996,7 +32306,7 @@
       <c r="V459" s="16"/>
       <c r="W459" s="16"/>
     </row>
-    <row r="460" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="460" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A460" s="5">
         <v>457</v>
       </c>
@@ -32061,7 +32371,7 @@
       <c r="V460" s="16"/>
       <c r="W460" s="16"/>
     </row>
-    <row r="461" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="461" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A461" s="5">
         <v>458</v>
       </c>
@@ -32124,7 +32434,7 @@
       <c r="V461" s="16"/>
       <c r="W461" s="16"/>
     </row>
-    <row r="462" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="462" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A462" s="5">
         <v>459</v>
       </c>
@@ -32187,7 +32497,7 @@
       <c r="V462" s="16"/>
       <c r="W462" s="16"/>
     </row>
-    <row r="463" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="463" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A463" s="5">
         <v>460</v>
       </c>
@@ -32250,7 +32560,7 @@
       <c r="V463" s="16"/>
       <c r="W463" s="16"/>
     </row>
-    <row r="464" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="464" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A464" s="5">
         <v>461</v>
       </c>
@@ -32313,7 +32623,7 @@
       <c r="V464" s="16"/>
       <c r="W464" s="16"/>
     </row>
-    <row r="465" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="465" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A465" s="5">
         <v>462</v>
       </c>
@@ -32378,7 +32688,7 @@
       <c r="V465" s="16"/>
       <c r="W465" s="16"/>
     </row>
-    <row r="466" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="466" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A466" s="5">
         <v>463</v>
       </c>
@@ -32443,7 +32753,7 @@
       <c r="V466" s="16"/>
       <c r="W466" s="16"/>
     </row>
-    <row r="467" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="467" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A467" s="5">
         <v>464</v>
       </c>
@@ -32506,7 +32816,7 @@
       <c r="V467" s="16"/>
       <c r="W467" s="16"/>
     </row>
-    <row r="468" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="468" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A468" s="5">
         <v>465</v>
       </c>
@@ -32569,7 +32879,7 @@
       <c r="V468" s="16"/>
       <c r="W468" s="16"/>
     </row>
-    <row r="469" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="469" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A469" s="5">
         <v>466</v>
       </c>
@@ -32634,7 +32944,7 @@
       <c r="V469" s="16"/>
       <c r="W469" s="16"/>
     </row>
-    <row r="470" spans="1:23" s="5" customFormat="1" ht="14.45" customHeight="1">
+    <row r="470" spans="1:23" s="5" customFormat="1" ht="14.4" customHeight="1">
       <c r="A470" s="5">
         <v>467</v>
       </c>
@@ -42978,7 +43288,7 @@
       </c>
       <c r="W633" s="20"/>
     </row>
-    <row r="634" spans="1:23" s="5" customFormat="1" ht="11.45" customHeight="1">
+    <row r="634" spans="1:23" s="5" customFormat="1" ht="11.4" customHeight="1">
       <c r="A634" s="5">
         <v>631</v>
       </c>
@@ -45074,4 +45384,585 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA3EAFE-03D4-4C4A-8C40-7704A7707EA7}">
+  <dimension ref="A1:AN6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:40">
+      <c r="A1" s="75" t="s">
+        <v>431</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>432</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>433</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>434</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>435</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>436</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>437</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>438</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>439</v>
+      </c>
+      <c r="J1" s="75" t="s">
+        <v>440</v>
+      </c>
+      <c r="K1" s="75" t="s">
+        <v>441</v>
+      </c>
+      <c r="L1" s="75" t="s">
+        <v>442</v>
+      </c>
+      <c r="M1" s="75" t="s">
+        <v>443</v>
+      </c>
+      <c r="N1" s="75" t="s">
+        <v>444</v>
+      </c>
+      <c r="O1" s="75" t="s">
+        <v>445</v>
+      </c>
+      <c r="P1" s="75" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q1" s="75" t="s">
+        <v>447</v>
+      </c>
+      <c r="R1" s="75" t="s">
+        <v>448</v>
+      </c>
+      <c r="S1" s="75" t="s">
+        <v>449</v>
+      </c>
+      <c r="T1" s="75" t="s">
+        <v>450</v>
+      </c>
+      <c r="U1" s="75" t="s">
+        <v>451</v>
+      </c>
+      <c r="V1" s="75" t="s">
+        <v>452</v>
+      </c>
+      <c r="W1" s="75" t="s">
+        <v>453</v>
+      </c>
+      <c r="X1" s="75" t="s">
+        <v>454</v>
+      </c>
+      <c r="Y1" s="75" t="s">
+        <v>455</v>
+      </c>
+      <c r="Z1" s="75" t="s">
+        <v>456</v>
+      </c>
+      <c r="AA1" s="75" t="s">
+        <v>457</v>
+      </c>
+      <c r="AB1" s="75" t="s">
+        <v>458</v>
+      </c>
+      <c r="AC1" s="75" t="s">
+        <v>459</v>
+      </c>
+      <c r="AD1" s="75" t="s">
+        <v>460</v>
+      </c>
+      <c r="AE1" s="75" t="s">
+        <v>461</v>
+      </c>
+      <c r="AF1" s="75" t="s">
+        <v>462</v>
+      </c>
+      <c r="AG1" s="75" t="s">
+        <v>463</v>
+      </c>
+      <c r="AH1" s="75" t="s">
+        <v>464</v>
+      </c>
+      <c r="AI1" s="75" t="s">
+        <v>465</v>
+      </c>
+      <c r="AJ1" s="75" t="s">
+        <v>466</v>
+      </c>
+      <c r="AK1" s="75" t="s">
+        <v>467</v>
+      </c>
+      <c r="AL1" s="75" t="s">
+        <v>468</v>
+      </c>
+      <c r="AM1" s="75" t="s">
+        <v>469</v>
+      </c>
+      <c r="AN1" s="75" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40">
+      <c r="A2" s="75" t="s">
+        <v>471</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>472</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>473</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>474</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>475</v>
+      </c>
+      <c r="F2" s="75" t="s">
+        <v>476</v>
+      </c>
+      <c r="G2" s="75" t="s">
+        <v>477</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>478</v>
+      </c>
+      <c r="I2" s="75" t="s">
+        <v>479</v>
+      </c>
+      <c r="J2" s="75" t="s">
+        <v>480</v>
+      </c>
+      <c r="K2" s="75" t="s">
+        <v>481</v>
+      </c>
+      <c r="L2" s="75" t="s">
+        <v>482</v>
+      </c>
+      <c r="M2" s="75" t="s">
+        <v>483</v>
+      </c>
+      <c r="N2" s="75" t="s">
+        <v>484</v>
+      </c>
+      <c r="O2" s="75" t="s">
+        <v>485</v>
+      </c>
+      <c r="P2" s="75" t="s">
+        <v>486</v>
+      </c>
+      <c r="Q2" s="75" t="s">
+        <v>487</v>
+      </c>
+      <c r="R2" s="75" t="s">
+        <v>488</v>
+      </c>
+      <c r="S2" s="75" t="s">
+        <v>489</v>
+      </c>
+      <c r="T2" s="75" t="s">
+        <v>490</v>
+      </c>
+      <c r="U2" s="75" t="s">
+        <v>491</v>
+      </c>
+      <c r="V2" s="75" t="s">
+        <v>492</v>
+      </c>
+      <c r="W2" s="75" t="s">
+        <v>493</v>
+      </c>
+      <c r="X2" s="75" t="s">
+        <v>494</v>
+      </c>
+      <c r="Y2" s="75" t="s">
+        <v>495</v>
+      </c>
+      <c r="Z2" s="75" t="s">
+        <v>496</v>
+      </c>
+      <c r="AA2" s="75" t="s">
+        <v>497</v>
+      </c>
+      <c r="AB2" s="75" t="s">
+        <v>498</v>
+      </c>
+      <c r="AC2" s="75" t="s">
+        <v>499</v>
+      </c>
+      <c r="AD2" s="75" t="s">
+        <v>500</v>
+      </c>
+      <c r="AE2" s="75" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF2" s="75" t="s">
+        <v>502</v>
+      </c>
+      <c r="AG2" s="75" t="s">
+        <v>503</v>
+      </c>
+      <c r="AH2" s="75" t="s">
+        <v>504</v>
+      </c>
+      <c r="AI2" s="75" t="s">
+        <v>505</v>
+      </c>
+      <c r="AJ2" s="75" t="s">
+        <v>506</v>
+      </c>
+      <c r="AK2" s="75" t="s">
+        <v>507</v>
+      </c>
+      <c r="AL2" s="75" t="s">
+        <v>508</v>
+      </c>
+      <c r="AM2" s="75" t="s">
+        <v>509</v>
+      </c>
+      <c r="AN2" s="75" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
+      <c r="A3" s="76" t="s">
+        <v>511</v>
+      </c>
+      <c r="B3" s="76" t="s">
+        <v>512</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>513</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>514</v>
+      </c>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76" t="s">
+        <v>417</v>
+      </c>
+      <c r="G3" s="76" t="s">
+        <v>515</v>
+      </c>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="K3" s="76" t="s">
+        <v>511</v>
+      </c>
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="76"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76" t="s">
+        <v>516</v>
+      </c>
+      <c r="Z3" s="76">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="76" t="s">
+        <v>517</v>
+      </c>
+      <c r="AB3" s="76" t="s">
+        <v>518</v>
+      </c>
+      <c r="AC3" s="76" t="s">
+        <v>519</v>
+      </c>
+      <c r="AD3" s="76">
+        <v>2019</v>
+      </c>
+      <c r="AE3" s="76" t="s">
+        <v>520</v>
+      </c>
+      <c r="AF3" s="76"/>
+      <c r="AG3" s="76"/>
+      <c r="AH3" s="76"/>
+      <c r="AI3" s="76"/>
+      <c r="AJ3" s="76"/>
+      <c r="AK3" s="76"/>
+      <c r="AL3" s="76"/>
+      <c r="AM3" s="76"/>
+      <c r="AN3" s="76"/>
+    </row>
+    <row r="4" spans="1:40">
+      <c r="A4" s="76" t="s">
+        <v>521</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>512</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76" t="s">
+        <v>417</v>
+      </c>
+      <c r="G4" s="76" t="s">
+        <v>419</v>
+      </c>
+      <c r="H4" s="76" t="s">
+        <v>523</v>
+      </c>
+      <c r="I4" s="76"/>
+      <c r="J4" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
+      <c r="M4" s="76"/>
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q4" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="R4" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="S4" s="76">
+        <v>1500</v>
+      </c>
+      <c r="T4" s="77">
+        <v>0.6</v>
+      </c>
+      <c r="U4" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="V4" s="76" t="s">
+        <v>525</v>
+      </c>
+      <c r="W4" s="76"/>
+      <c r="X4" s="76"/>
+      <c r="Y4" s="76"/>
+      <c r="Z4" s="76"/>
+      <c r="AA4" s="76"/>
+      <c r="AB4" s="76"/>
+      <c r="AC4" s="76"/>
+      <c r="AD4" s="76"/>
+      <c r="AE4" s="76" t="s">
+        <v>526</v>
+      </c>
+      <c r="AF4" s="76"/>
+      <c r="AG4" s="76"/>
+      <c r="AH4" s="76"/>
+      <c r="AI4" s="76"/>
+      <c r="AJ4" s="76"/>
+      <c r="AK4" s="76"/>
+      <c r="AL4" s="76"/>
+      <c r="AM4" s="76"/>
+      <c r="AN4" s="76"/>
+    </row>
+    <row r="5" spans="1:40">
+      <c r="A5" s="76" t="s">
+        <v>427</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>512</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>417</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>419</v>
+      </c>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="76"/>
+      <c r="L5" s="76"/>
+      <c r="M5" s="76"/>
+      <c r="N5" s="76"/>
+      <c r="O5" s="76"/>
+      <c r="P5" s="76"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="76"/>
+      <c r="S5" s="76"/>
+      <c r="T5" s="76"/>
+      <c r="U5" s="76"/>
+      <c r="V5" s="76" t="s">
+        <v>525</v>
+      </c>
+      <c r="W5" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="X5" s="76" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="Z5" s="76">
+        <v>1500</v>
+      </c>
+      <c r="AA5" s="77">
+        <v>0.6</v>
+      </c>
+      <c r="AB5" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="AC5" s="76"/>
+      <c r="AD5" s="76"/>
+      <c r="AE5" s="76"/>
+      <c r="AF5" s="77">
+        <v>0.85</v>
+      </c>
+      <c r="AG5" s="76"/>
+      <c r="AH5" s="76" t="s">
+        <v>527</v>
+      </c>
+      <c r="AI5" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ5" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK5" s="76">
+        <v>11</v>
+      </c>
+      <c r="AL5" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM5" s="76"/>
+      <c r="AN5" s="76"/>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="A6" s="76" t="s">
+        <v>528</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>512</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>522</v>
+      </c>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76" t="s">
+        <v>417</v>
+      </c>
+      <c r="G6" s="76" t="s">
+        <v>419</v>
+      </c>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76" t="s">
+        <v>146</v>
+      </c>
+      <c r="K6" s="76" t="s">
+        <v>529</v>
+      </c>
+      <c r="L6" s="76" t="s">
+        <v>232</v>
+      </c>
+      <c r="M6" s="76" t="s">
+        <v>232</v>
+      </c>
+      <c r="N6" s="76" t="s">
+        <v>232</v>
+      </c>
+      <c r="O6" s="76" t="s">
+        <v>232</v>
+      </c>
+      <c r="P6" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q6" s="76" t="s">
+        <v>524</v>
+      </c>
+      <c r="R6" s="77">
+        <v>0.1</v>
+      </c>
+      <c r="S6" s="76">
+        <v>1500</v>
+      </c>
+      <c r="T6" s="77">
+        <v>0.6</v>
+      </c>
+      <c r="U6" s="76" t="s">
+        <v>518</v>
+      </c>
+      <c r="V6" s="76" t="s">
+        <v>525</v>
+      </c>
+      <c r="W6" s="76"/>
+      <c r="X6" s="76"/>
+      <c r="Y6" s="76"/>
+      <c r="Z6" s="76"/>
+      <c r="AA6" s="76"/>
+      <c r="AB6" s="76"/>
+      <c r="AC6" s="76"/>
+      <c r="AD6" s="76"/>
+      <c r="AE6" s="76"/>
+      <c r="AF6" s="77">
+        <v>0.85</v>
+      </c>
+      <c r="AG6" s="76"/>
+      <c r="AH6" s="76" t="s">
+        <v>527</v>
+      </c>
+      <c r="AI6" s="76" t="s">
+        <v>159</v>
+      </c>
+      <c r="AJ6" s="76" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK6" s="76">
+        <v>12</v>
+      </c>
+      <c r="AL6" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="AM6" s="76"/>
+      <c r="AN6" s="76"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>